<commit_message>
update chisquare test added
</commit_message>
<xml_diff>
--- a/2017-2018 data set.xlsx
+++ b/2017-2018 data set.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nana Dom\IdeaProjects\A-Comparative-Statistical-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010CB8D2-3B1B-45E4-A892-CD842ACE29DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3799AB-824B-4A64-9C84-6B77670C0654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{4290AEC0-4F1B-450C-BFC0-53A45CD5E5C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{4290AEC0-4F1B-450C-BFC0-53A45CD5E5C3}"/>
   </bookViews>
   <sheets>
     <sheet name="17-18" sheetId="1" r:id="rId1"/>
     <sheet name="2024" sheetId="3" r:id="rId2"/>
+    <sheet name="2024-figures" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="12">
   <si>
     <t>Male</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>Locality</t>
+  </si>
+  <si>
+    <t>Education</t>
   </si>
 </sst>
 </file>
@@ -130,19 +134,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B9AF0-E966-4931-AD5D-B18A0011E4C8}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +507,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
@@ -508,10 +522,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -523,10 +537,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -538,10 +552,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -554,10 +568,10 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -570,10 +584,10 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -586,10 +600,10 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -602,10 +616,10 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -618,10 +632,10 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -634,10 +648,10 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -650,10 +664,10 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -672,18 +686,18 @@
       <c r="F13" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -720,10 +734,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
@@ -735,10 +749,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -750,10 +764,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -765,10 +779,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -781,10 +795,10 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -797,10 +811,10 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -813,10 +827,10 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,10 +843,10 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -845,10 +859,10 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -861,10 +875,10 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -877,10 +891,10 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -899,33 +913,364 @@
       <c r="F13" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E560E7-BB4D-4529-B98D-BDB38AC7A3C6}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6">
+        <f>SUM(C4,C6,C8,C10)</f>
+        <v>470298</v>
+      </c>
+      <c r="D2" s="6">
+        <f>SUM(D4,D6,D8,D10)</f>
+        <v>231884</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <f>SUM(C5,C7,C9,C11)</f>
+        <v>1514244</v>
+      </c>
+      <c r="D3" s="6">
+        <f>SUM(D5,D7,D9,D11)</f>
+        <v>803343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>121791</v>
+      </c>
+      <c r="D4" s="6">
+        <v>90138</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>632508</v>
+      </c>
+      <c r="D5" s="6">
+        <v>439349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>218916</v>
+      </c>
+      <c r="D6" s="6">
+        <v>114114</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>691403</v>
+      </c>
+      <c r="D7" s="6">
+        <v>324433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6">
+        <v>77217</v>
+      </c>
+      <c r="D8" s="6">
+        <v>19898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6">
+        <v>138112</v>
+      </c>
+      <c r="D9" s="6">
+        <v>32904</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6">
+        <v>52374</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>52221</v>
+      </c>
+      <c r="D11" s="6">
+        <v>6657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>